<commit_message>
4o not told about number of players
</commit_message>
<xml_diff>
--- a/common_auction_data.xlsx
+++ b/common_auction_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CS\LLMauctions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21635C87-180B-42D0-91EE-83A92BA2B69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A11137-B3B4-4FBE-BEE1-50A0C09B7D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{3A177D61-6A2A-49C9-8862-9F5BFBF29A16}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{3A177D61-6A2A-49C9-8862-9F5BFBF29A16}"/>
   </bookViews>
   <sheets>
     <sheet name="GPT-4o" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="17">
   <si>
     <t>Round 1</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Not told 10</t>
+  </si>
+  <si>
+    <t>Not told 10 players</t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D852F3E-2B2F-4BC0-8AE0-9D40EC0F1D32}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -981,12 +984,215 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
       <c r="M14">
         <f>AVERAGE(L2:L12)</f>
         <v>21.272727272727273</v>
       </c>
     </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>21</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>12</v>
+      </c>
+      <c r="J15">
+        <v>12</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>13</v>
+      </c>
+      <c r="H16">
+        <v>12</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>15</v>
+      </c>
+      <c r="K17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>13</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>13</v>
+      </c>
+      <c r="H19">
+        <v>14</v>
+      </c>
+      <c r="I19">
+        <v>12</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -995,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9315AC-6FDC-4F88-878A-9DCC99BF6B1A}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
gemini at a common auction
</commit_message>
<xml_diff>
--- a/common_auction_data.xlsx
+++ b/common_auction_data.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CS\LLMauctions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A11137-B3B4-4FBE-BEE1-50A0C09B7D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9922EA35-51B6-46CF-B6F4-417A6F7E0A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{3A177D61-6A2A-49C9-8862-9F5BFBF29A16}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{3A177D61-6A2A-49C9-8862-9F5BFBF29A16}"/>
   </bookViews>
   <sheets>
     <sheet name="GPT-4o" sheetId="1" r:id="rId1"/>
-    <sheet name="Claude Sonnet 3.5" sheetId="2" r:id="rId2"/>
+    <sheet name="Gemini-1.5-Flash" sheetId="3" r:id="rId2"/>
+    <sheet name="Gemini-1.5-Pro" sheetId="4" r:id="rId3"/>
+    <sheet name="Claude Sonnet 3.5" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="16">
   <si>
     <t>Round 1</t>
   </si>
@@ -75,9 +77,6 @@
     <t>Round 11</t>
   </si>
   <si>
-    <t>Round 12</t>
-  </si>
-  <si>
     <t>Told 10 players</t>
   </si>
   <si>
@@ -109,18 +108,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -135,9 +128,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,15 +466,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D852F3E-2B2F-4BC0-8AE0-9D40EC0F1D32}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -516,42 +508,42 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>6</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <f>SUM(B2:K2)</f>
-        <v>33</v>
+        <f t="shared" ref="L2:L25" si="0">SUM(B2:K2)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -559,194 +551,194 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3">
         <v>5</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
       <c r="L3">
-        <f t="shared" ref="L3:L13" si="0">SUM(B3:K3)</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
       </c>
       <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
       </c>
       <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="K5" t="s">
+        <v>4</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>1</v>
+      <c r="B6" t="s">
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
-        <v>4</v>
+      <c r="E6">
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>3</v>
-      </c>
-      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>4</v>
       </c>
       <c r="J6">
-        <v>5</v>
-      </c>
-      <c r="K6" t="s">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
       </c>
       <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
         <v>5</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>4</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -756,17 +748,17 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -774,57 +766,57 @@
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
+      <c r="I8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" t="s">
+        <v>4</v>
       </c>
       <c r="K8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>0</v>
+      <c r="B9" t="s">
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
         <v>6</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>7</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" t="s">
-        <v>4</v>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -835,74 +827,74 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
         <v>5</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-      <c r="G10">
-        <v>6</v>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
+      <c r="B11">
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
         <v>4</v>
       </c>
-      <c r="G11" t="s">
-        <v>4</v>
+      <c r="G11">
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -910,22 +902,22 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -937,258 +929,456 @@
         <v>1</v>
       </c>
       <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
         <v>7</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f>AVERAGE(L2:L11)</f>
+        <v>20.100000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="M14">
-        <f>AVERAGE(L2:L12)</f>
-        <v>21.272727272727273</v>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>21</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+      <c r="J14">
+        <v>12</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B15">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
         <v>13</v>
-      </c>
-      <c r="E15">
-        <v>21</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
       </c>
       <c r="H15">
         <v>12</v>
       </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
       <c r="J15">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>15</v>
+      </c>
+      <c r="K16">
+        <v>14</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>13</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
         <v>5</v>
       </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
+      <c r="G18">
         <v>13</v>
       </c>
-      <c r="H16">
+      <c r="H18">
+        <v>14</v>
+      </c>
+      <c r="I18">
         <v>12</v>
       </c>
-      <c r="I16">
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>15</v>
-      </c>
-      <c r="K17">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18">
-        <v>15</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>14</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="H19">
+        <v>17</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>16</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
         <v>13</v>
       </c>
-      <c r="I18">
-        <v>3</v>
-      </c>
-      <c r="J18">
-        <v>3</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <v>15</v>
-      </c>
-      <c r="E19">
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="F19">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>12</v>
+      </c>
+      <c r="I21">
+        <v>16</v>
+      </c>
+      <c r="J21">
+        <v>17</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
         <v>5</v>
       </c>
-      <c r="G19">
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>9</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>8</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>16</v>
+      </c>
+      <c r="D24">
         <v>13</v>
       </c>
-      <c r="H19">
-        <v>14</v>
-      </c>
-      <c r="I19">
+      <c r="E24">
+        <v>17</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>13</v>
+      </c>
+      <c r="H24">
+        <v>13</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
         <v>12</v>
       </c>
-      <c r="J19">
-        <v>3</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>10</v>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M25">
+        <f>AVERAGE(L14:L24)</f>
+        <v>58.363636363636367</v>
       </c>
     </row>
   </sheetData>
@@ -1198,18 +1388,1697 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E3E645-EF8E-40B2-91A0-7B0913EC63F3}">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L22" si="0">SUM(B2:K2)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F269E38A-FF07-41EE-A108-FA417E4C7025}">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L22" si="0">SUM(B2:K2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9315AC-6FDC-4F88-878A-9DCC99BF6B1A}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -1244,7 +3113,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -1673,7 +3542,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
@@ -1686,7 +3555,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -1801,7 +3670,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1840,7 +3709,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1879,7 +3748,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1918,7 +3787,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1957,7 +3826,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1996,7 +3865,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2035,7 +3904,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -2074,7 +3943,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2111,6 +3980,12 @@
       <c r="L24">
         <f t="shared" si="0"/>
         <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M25">
+        <f>AVERAGE(L14:L24)</f>
+        <v>221.90909090909091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4o and 4o-mini at an english auction
</commit_message>
<xml_diff>
--- a/common_auction_data.xlsx
+++ b/common_auction_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CS\LLMauctions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9922EA35-51B6-46CF-B6F4-417A6F7E0A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA73D421-50E8-4E78-B32E-7E7D14F44D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{3A177D61-6A2A-49C9-8862-9F5BFBF29A16}"/>
+    <workbookView xWindow="5760" yWindow="720" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{3A177D61-6A2A-49C9-8862-9F5BFBF29A16}"/>
   </bookViews>
   <sheets>
     <sheet name="GPT-4o" sheetId="1" r:id="rId1"/>
@@ -1392,7 +1392,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L22"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1825,10 +1825,6 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2231,8 +2227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F269E38A-FF07-41EE-A108-FA417E4C7025}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2665,10 +2661,6 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -3070,8 +3062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9315AC-6FDC-4F88-878A-9DCC99BF6B1A}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>